<commit_message>
added tasks. Tick for done,cross for not done
</commit_message>
<xml_diff>
--- a/TaskSchedule.xlsx
+++ b/TaskSchedule.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yfazla1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LSU\Spring 2017\Game Design\CSC4263-ART4240\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="63">
   <si>
     <t>Remainning Task</t>
   </si>
@@ -207,19 +207,31 @@
   </si>
   <si>
     <t>Camera Moving</t>
+  </si>
+  <si>
+    <t>√</t>
+  </si>
+  <si>
+    <t>×</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -330,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -338,6 +350,54 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -347,64 +407,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -428,6 +458,60 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1257300</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>271462</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5943600" y="13473112"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -696,7 +780,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -735,344 +819,462 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F2" s="26" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="F3" s="26" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F4" s="26" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F5" s="26" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="F6" s="26" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="7" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="F7" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" s="7" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="7" t="s">
+      <c r="D8" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" s="7" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="7" t="s">
+      <c r="D9" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" s="7" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="6" t="s">
+      <c r="D10" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" s="7" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="7" t="s">
+      <c r="E11" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" s="7" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="6" t="s">
+      <c r="G12" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" s="7" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="7" t="s">
+      <c r="G13" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="G14" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="12" t="s">
+      <c r="F15" s="28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="10" t="s">
+      <c r="F16" s="28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="12" t="s">
+    <row r="18" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="12" t="s">
+    <row r="19" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
+      <c r="B19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="12" t="s">
+      <c r="H19" s="28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="12" t="s">
+      <c r="H20" s="28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="12" t="s">
+      <c r="D21" s="28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
+      <c r="B22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="12" t="s">
+    <row r="23" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="B23" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="10" t="s">
+    <row r="24" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+      <c r="B24" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="12" t="s">
+      <c r="F24" s="28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="16" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+    <row r="26" spans="1:8" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" s="16" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="16" t="s">
+      <c r="G26" s="30"/>
+      <c r="H26" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" s="16" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="16" t="s">
+      <c r="H27" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" s="16" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="16" t="s">
+      <c r="H28" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" s="16" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="16" t="s">
+      <c r="H29" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" s="16" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="16" t="s">
+      <c r="H30" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" s="20" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
+      <c r="H31" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="7" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" s="20" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
-      <c r="B33" s="20" t="s">
+      <c r="C32" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="31"/>
+    </row>
+    <row r="33" spans="1:8" s="7" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
+      <c r="B33" s="7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" s="23" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
+      <c r="C33" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="23" t="s">
+      <c r="C34" s="8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" s="23" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="23" t="s">
+      <c r="D34" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="29"/>
+    </row>
+    <row r="35" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" s="23" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="23" t="s">
+      <c r="G35" s="29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="23" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="23" t="s">
+    <row r="37" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="8" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" s="23" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
-      <c r="B38" s="22" t="s">
+      <c r="D37" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" s="23" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="23" t="s">
+      <c r="F38" s="29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" s="23" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
-      <c r="B40" s="22" t="s">
+      <c r="G39" s="29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="B40" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" s="23" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="23" t="s">
+      <c r="D40" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" s="23" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
-      <c r="B42" s="23" t="s">
+      <c r="D41" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="B42" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="23" t="s">
+      <c r="C42" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" s="23" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
-      <c r="B43" s="23" t="s">
+      <c r="D42" s="29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="23" t="s">
+      <c r="C43" s="8" t="s">
         <v>56</v>
+      </c>
+      <c r="H43" s="29" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A15:A25"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A14"/>
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="A34:A43"/>
     <mergeCell ref="A26:A31"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="B34:B37"/>
     <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A15:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the work done
</commit_message>
<xml_diff>
--- a/TaskSchedule.xlsx
+++ b/TaskSchedule.xlsx
@@ -368,6 +368,51 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -390,51 +435,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -779,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -819,174 +819,174 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="9" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="9" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="27" t="s">
-        <v>62</v>
+      <c r="D8" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="18"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="27" t="s">
+      <c r="D9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="27" t="s">
+      <c r="D10" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="17" t="s">
+      <c r="A11" s="23"/>
+      <c r="B11" s="18" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="17" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="18" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="24"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="23" t="s">
+      <c r="A17" s="17"/>
+      <c r="B17" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -994,47 +994,47 @@
       </c>
     </row>
     <row r="18" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="24"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="28" t="s">
-        <v>62</v>
+      <c r="D21" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="5" t="s">
         <v>29</v>
       </c>
@@ -1043,143 +1043,142 @@
       </c>
     </row>
     <row r="23" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="23" t="s">
+      <c r="A24" s="17"/>
+      <c r="B24" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="27" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30" t="s">
+      <c r="G26" s="13"/>
+      <c r="H26" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H27" s="30" t="s">
+      <c r="H27" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H28" s="30" t="s">
+      <c r="H28" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H29" s="30" t="s">
+      <c r="H29" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H30" s="30" t="s">
+      <c r="H30" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H31" s="30" t="s">
+      <c r="H31" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="7" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="30" t="s">
         <v>44</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32" s="31"/>
+      <c r="D32" s="14" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="33" spans="1:8" s="7" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
+      <c r="A33" s="31"/>
       <c r="B33" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="D33" s="14" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="24" t="s">
         <v>17</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="29" t="s">
+      <c r="D34" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="29"/>
+      <c r="E34" s="12"/>
     </row>
     <row r="35" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
       <c r="C35" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G35" s="29" t="s">
+      <c r="G35" s="12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
       <c r="C36" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="25"/>
       <c r="C37" s="8" t="s">
         <v>55</v>
       </c>
@@ -1188,42 +1187,42 @@
       </c>
     </row>
     <row r="38" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
-      <c r="B38" s="9" t="s">
+      <c r="A38" s="26"/>
+      <c r="B38" s="24" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F38" s="29" t="s">
+      <c r="F38" s="12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="10"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="25"/>
       <c r="C39" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G39" s="29" t="s">
+      <c r="G39" s="12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
-      <c r="B40" s="9" t="s">
+      <c r="A40" s="26"/>
+      <c r="B40" s="24" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>56</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="10"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="25"/>
       <c r="C41" s="8" t="s">
         <v>58</v>
       </c>
@@ -1232,38 +1231,31 @@
       </c>
     </row>
     <row r="42" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="8" t="s">
         <v>59</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D42" s="29" t="s">
+      <c r="D42" s="12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H43" s="29" t="s">
+      <c r="H43" s="12" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A15:A25"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A14"/>
     <mergeCell ref="B40:B41"/>
@@ -1272,6 +1264,13 @@
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="B34:B37"/>
     <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A15:A25"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>